<commit_message>
withdrawaremoved ConfigMgr and added PriceRequester. All tsts okl testing ok
</commit_message>
<xml_diff>
--- a/test/testdata/testSBEarningUsdc_uniqueOwner_1_deposit_1_almost_full_withdr_fixed_yield_rate.xlsx
+++ b/test/testdata/testSBEarningUsdc_uniqueOwner_1_deposit_1_almost_full_withdr_fixed_yield_rate.xlsx
@@ -478,10 +478,10 @@
     <xf numFmtId="168" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,19 +853,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="9" spans="1:11" ht="26.15" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="5">
-        <v>10.007703465398601</v>
+        <v>4.9929284661399996E-3</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="4" t="s">
@@ -2160,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="5">
-        <v>1.249131575827E-2</v>
+        <v>4.9979190050799998E-3</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="4" t="s">
@@ -2168,9 +2168,9 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="I47" s="12">
+      <c r="I47" s="11">
         <f>SUM(I42:I46)</f>
-        <v>40.013328894451078</v>
+        <v>30.003124960765433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>